<commit_message>
BIS-1630: Fixed eln-template-types import xls file
</commit_message>
<xml_diff>
--- a/core-plugin-openbis/dist/core-plugins/eln-lims-template-types/2/as/master-data/eln-types-template.xlsx
+++ b/core-plugin-openbis/dist/core-plugins/eln-lims-template-types/2/as/master-data/eln-types-template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="103">
   <si>
     <t xml:space="preserve">SAMPLE_TYPE</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mandatory</t>
   </si>
   <si>
@@ -77,9 +80,6 @@
   </si>
   <si>
     <t xml:space="preserve">NAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
   </si>
   <si>
     <t xml:space="preserve">General info</t>
@@ -465,7 +465,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,8 +508,8 @@
   </sheetPr>
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -576,9 +576,8 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="D3" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>7</v>
@@ -592,50 +591,48 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>20</v>
@@ -658,15 +655,13 @@
         <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>20</v>
@@ -689,15 +684,13 @@
         <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>20</v>
@@ -764,9 +757,8 @@
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="D11" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>32</v>
@@ -783,50 +775,48 @@
         <v>2</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>20</v>
@@ -849,15 +839,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>20</v>
@@ -880,15 +868,13 @@
         <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>20</v>
@@ -916,13 +902,11 @@
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>20</v>
@@ -947,13 +931,11 @@
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>20</v>
@@ -978,13 +960,11 @@
       <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>20</v>
@@ -1009,13 +989,11 @@
       <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>48</v>
@@ -1043,13 +1021,11 @@
       <c r="B20" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D20" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>48</v>
@@ -1077,13 +1053,11 @@
       <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>48</v>
@@ -1111,13 +1085,11 @@
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>48</v>
@@ -1145,13 +1117,11 @@
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>63</v>
@@ -1179,13 +1149,11 @@
       <c r="B24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>63</v>
@@ -1213,13 +1181,11 @@
       <c r="B25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D25" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>69</v>
@@ -1245,15 +1211,13 @@
         <v>71</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="4" t="s">
@@ -1321,50 +1285,48 @@
         <v>2</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D32" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>20</v>
@@ -1387,15 +1349,13 @@
         <v>75</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>20</v>
@@ -1418,15 +1378,13 @@
         <v>23</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D34" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>20</v>
@@ -1449,15 +1407,13 @@
         <v>78</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>20</v>
@@ -1485,13 +1441,11 @@
       <c r="B36" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D36" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>20</v>
@@ -1516,13 +1470,11 @@
       <c r="B37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E37" s="0" t="s">
         <v>20</v>
@@ -1547,13 +1499,11 @@
       <c r="B38" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D38" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>20</v>
@@ -1578,13 +1528,11 @@
       <c r="B39" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D39" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E39" s="0" t="s">
         <v>20</v>
@@ -1609,13 +1557,11 @@
       <c r="B40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>48</v>
@@ -1643,13 +1589,11 @@
       <c r="B41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D41" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E41" s="0" t="s">
         <v>48</v>
@@ -1677,13 +1621,11 @@
       <c r="B42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D42" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E42" s="0" t="s">
         <v>48</v>
@@ -1711,13 +1653,11 @@
       <c r="B43" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D43" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>63</v>
@@ -1745,13 +1685,11 @@
       <c r="B44" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D44" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>63</v>
@@ -1779,13 +1717,11 @@
       <c r="B45" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D45" s="5" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4" t="s">
@@ -1809,15 +1745,13 @@
         <v>71</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D46" s="5" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>69</v>

</xml_diff>